<commit_message>
Evolution du gabarit ACA en indice "C"
</commit_message>
<xml_diff>
--- a/ACA tool palettes/FRA/Gabarit ACA/Evolution du gabarit ACA.xlsx
+++ b/ACA tool palettes/FRA/Gabarit ACA/Evolution du gabarit ACA.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin Marquette\Documents\GitHub\BetaProgram\ACA tool palettes\FRA\Gabarit ACA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE76D54-63F5-4910-B7BE-F49DF3F3E34D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F73E1E-32B9-4F29-8B75-A689C6C2A607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17596" xr2:uid="{A80ABF4B-E54B-4375-B72F-5407CCC93B9D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="General" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>_C3D-TEMPLATE_2025_FRA (Architecture v0001a)</t>
   </si>
@@ -47,16 +47,41 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Ajout des hachures 2D (vue de dessus) pour les masses élémentaires (style Standard)</t>
-  </si>
-  <si>
     <t>Evolution du gabarit ACA</t>
   </si>
   <si>
     <t>Nom de la version</t>
   </si>
   <si>
-    <t>Prise en compte des vues 3D pour les objets traditionnels de construction (murs, toits, dalles, etc.)</t>
+    <t>Prise en compte des vues 3D pour les objets traditionnels de construction (paramétrages des murs, toits, dalles, etc.)</t>
+  </si>
+  <si>
+    <t>Ajout des hachures 2D (vue de dessus) pour les masses élémentaires (modification du style Standard présent par défaut)</t>
+  </si>
+  <si>
+    <t>_C3D-TEMPLATE_2025_FRA (Architecture v0001c)</t>
+  </si>
+  <si>
+    <t>Ajout d'un style Standard ACA pour les objets architecturaux suivants : 
+- Définitions de formes d'éléments de structure ;
+- Définitions des groupes de nettoyage de murs ;
+- Styles de blocs porte/fenêtre ;
+- Styles de bords de dalle ;
+- Styles de bords de dalle du toit ;
+- Styles de dalles ;
+- Styles de dalles du toit ;
+- Styles de fenêtres ;
+- Styles de garde-corps ;
+- Styles de murs ;
+- Styles de murs-rideaux ;
+- Styles de portes ;
+- Styles d'escaliers ;
+- Styles d'espaces (avec en supplément les styles Commerce, Education, Habitation, Logement, Santé) ;
+- Styles d'extrémités de mur ;
+- Styles d'extrémités d'ouverture de mur ;
+- Styles d'unités de mur-rideau.
+L'implémentation de ces styles Standard ACA dans le gabarit empêche Civil 3D de créer ses propres styles Standard par défaut qui seraient mal paramétrés ou avec des composants manquants dans l'affichage (les rambardes des garde-corps par exemple).
+Les styles de balancements d'escaliers Equilibré, Manuel, Sur un point sont également implémentés dans cette nouvelle version du gabarit.</t>
   </si>
 </sst>
 </file>
@@ -124,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -137,6 +162,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -472,27 +503,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D13BAD-6F1A-48D2-A554-8EAC8DE81690}">
-  <dimension ref="B2:C6"/>
+  <dimension ref="B2:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
     <col min="2" max="2" width="43.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="80" style="2" customWidth="1"/>
+    <col min="3" max="3" width="113.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B4" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
@@ -503,7 +534,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.45">
@@ -511,7 +542,15 @@
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>3</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="299.25" x14ac:dyDescent="0.45">
+      <c r="B7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Evolution gabarit ACA indice "D"
</commit_message>
<xml_diff>
--- a/ACA tool palettes/FRA/Gabarit ACA/Evolution du gabarit ACA.xlsx
+++ b/ACA tool palettes/FRA/Gabarit ACA/Evolution du gabarit ACA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin Marquette\Documents\GitHub\BetaProgram\ACA tool palettes\FRA\Gabarit ACA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F73E1E-32B9-4F29-8B75-A689C6C2A607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A078404-B87D-4872-9952-9480C033A6D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17596" xr2:uid="{A80ABF4B-E54B-4375-B72F-5407CCC93B9D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>_C3D-TEMPLATE_2025_FRA (Architecture v0001a)</t>
   </si>
@@ -82,6 +82,12 @@
 - Styles d'unités de mur-rideau.
 L'implémentation de ces styles Standard ACA dans le gabarit empêche Civil 3D de créer ses propres styles Standard par défaut qui seraient mal paramétrés ou avec des composants manquants dans l'affichage (les rambardes des garde-corps par exemple).
 Les styles de balancements d'escaliers Equilibré, Manuel, Sur un point sont également implémentés dans cette nouvelle version du gabarit.</t>
+  </si>
+  <si>
+    <t>_C3D-TEMPLATE_2025_FRA (Architecture v0001d)</t>
+  </si>
+  <si>
+    <t>Ecrase le style dalle indice C pour le remplacer par le style dalle indice B (perte des jeux automatiques de propriétés)</t>
   </si>
 </sst>
 </file>
@@ -503,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D13BAD-6F1A-48D2-A554-8EAC8DE81690}">
-  <dimension ref="B2:C7"/>
+  <dimension ref="B2:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -553,6 +559,14 @@
         <v>8</v>
       </c>
     </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Evolution du gabarit ACA en indice "D"(re-upload)
</commit_message>
<xml_diff>
--- a/ACA tool palettes/FRA/Gabarit ACA/Evolution du gabarit ACA.xlsx
+++ b/ACA tool palettes/FRA/Gabarit ACA/Evolution du gabarit ACA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin Marquette\Documents\GitHub\BetaProgram\ACA tool palettes\FRA\Gabarit ACA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A078404-B87D-4872-9952-9480C033A6D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0DE9BC1-1D52-4A8D-B814-1B4693258C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17596" xr2:uid="{A80ABF4B-E54B-4375-B72F-5407CCC93B9D}"/>
+    <workbookView xWindow="2835" yWindow="9090" windowWidth="24300" windowHeight="6577" xr2:uid="{A80ABF4B-E54B-4375-B72F-5407CCC93B9D}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -87,7 +87,7 @@
     <t>_C3D-TEMPLATE_2025_FRA (Architecture v0001d)</t>
   </si>
   <si>
-    <t>Ecrase le style dalle indice C pour le remplacer par le style dalle indice B (perte des jeux automatiques de propriétés)</t>
+    <t>Annulation du remplacement de style en mode Plan (pour revenir à Dessin par défaut) et récupérer le hachurage en vue 2D de dessus</t>
   </si>
 </sst>
 </file>
@@ -511,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D13BAD-6F1A-48D2-A554-8EAC8DE81690}">
   <dimension ref="B2:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Evolution du gabarit ACA en indice "E"
</commit_message>
<xml_diff>
--- a/ACA tool palettes/FRA/Gabarit ACA/Evolution du gabarit ACA.xlsx
+++ b/ACA tool palettes/FRA/Gabarit ACA/Evolution du gabarit ACA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin Marquette\Documents\GitHub\BetaProgram\ACA tool palettes\FRA\Gabarit ACA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0DE9BC1-1D52-4A8D-B814-1B4693258C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9FB719E-E0D4-4CCC-943D-7C0F4072941B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2835" yWindow="9090" windowWidth="24300" windowHeight="6577" xr2:uid="{A80ABF4B-E54B-4375-B72F-5407CCC93B9D}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17596" xr2:uid="{A80ABF4B-E54B-4375-B72F-5407CCC93B9D}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>_C3D-TEMPLATE_2025_FRA (Architecture v0001a)</t>
   </si>
@@ -88,6 +88,18 @@
   </si>
   <si>
     <t>Annulation du remplacement de style en mode Plan (pour revenir à Dessin par défaut) et récupérer le hachurage en vue 2D de dessus</t>
+  </si>
+  <si>
+    <t>_C3D-TEMPLATE_2025_FRA (Architecture v0001e)</t>
+  </si>
+  <si>
+    <t>Ajout d'un style Standard ACA pour les objets de documentation suivants : 
+- Gabarits de zone ;
+- Styles de cotes AEC ;
+- Styles de zones ;
+- Styles d'élévations/de coupes 2D ;
+- Styles des thèmes d'affichage.
+L'implémentation de ces styles Standard ACA dans le gabarit empêche Civil 3D de créer ses propres styles Standard par défaut qui seraient mal paramétrés.</t>
   </si>
 </sst>
 </file>
@@ -509,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D13BAD-6F1A-48D2-A554-8EAC8DE81690}">
-  <dimension ref="B2:C8"/>
+  <dimension ref="B2:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -567,6 +579,14 @@
         <v>10</v>
       </c>
     </row>
+    <row r="9" spans="2:3" ht="114" x14ac:dyDescent="0.45">
+      <c r="B9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Evolution du gabarit ACA en indice "F"
</commit_message>
<xml_diff>
--- a/ACA tool palettes/FRA/Gabarit ACA/Evolution du gabarit ACA.xlsx
+++ b/ACA tool palettes/FRA/Gabarit ACA/Evolution du gabarit ACA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin Marquette\Documents\GitHub\BetaProgram\ACA tool palettes\FRA\Gabarit ACA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9FB719E-E0D4-4CCC-943D-7C0F4072941B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90F1B31-0399-41AF-976C-134651525ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17596" xr2:uid="{A80ABF4B-E54B-4375-B72F-5407CCC93B9D}"/>
+    <workbookView xWindow="11415" yWindow="518" windowWidth="24300" windowHeight="15157" xr2:uid="{A80ABF4B-E54B-4375-B72F-5407CCC93B9D}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>_C3D-TEMPLATE_2025_FRA (Architecture v0001a)</t>
   </si>
@@ -100,6 +100,23 @@
 - Styles d'élévations/de coupes 2D ;
 - Styles des thèmes d'affichage.
 L'implémentation de ces styles Standard ACA dans le gabarit empêche Civil 3D de créer ses propres styles Standard par défaut qui seraient mal paramétrés.</t>
+  </si>
+  <si>
+    <t>_C3D-TEMPLATE_2025_FRA (Architecture v0001f)</t>
+  </si>
+  <si>
+    <t>Ajout des Définitions des jeux de propriétés suivants : 
+- BlocPorteFenetre ;
+- Dalle ;
+- ElementStructure ;
+- Escalier ;
+- Espace ;
+- Fenetre ;
+- Mur ; 
+- MurRideau ; 
+- MurRideau-Style ;
+- Mur-Style ;
+- Porte.</t>
   </si>
 </sst>
 </file>
@@ -521,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D13BAD-6F1A-48D2-A554-8EAC8DE81690}">
-  <dimension ref="B2:C9"/>
+  <dimension ref="B2:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -587,6 +604,14 @@
         <v>12</v>
       </c>
     </row>
+    <row r="10" spans="2:3" ht="171" x14ac:dyDescent="0.45">
+      <c r="B10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Evolution du gabarit ACA en indice "G"
</commit_message>
<xml_diff>
--- a/ACA tool palettes/FRA/Gabarit ACA/Evolution du gabarit ACA.xlsx
+++ b/ACA tool palettes/FRA/Gabarit ACA/Evolution du gabarit ACA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin Marquette\Documents\GitHub\BetaProgram\ACA tool palettes\FRA\Gabarit ACA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90F1B31-0399-41AF-976C-134651525ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D6A6DF-A18F-4385-A244-0021F42F96BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11415" yWindow="518" windowWidth="24300" windowHeight="15157" xr2:uid="{A80ABF4B-E54B-4375-B72F-5407CCC93B9D}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17596" xr2:uid="{A80ABF4B-E54B-4375-B72F-5407CCC93B9D}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>_C3D-TEMPLATE_2025_FRA (Architecture v0001a)</t>
   </si>
@@ -117,6 +117,14 @@
 - MurRideau-Style ;
 - Mur-Style ;
 - Porte.</t>
+  </si>
+  <si>
+    <t>_C3D-TEMPLATE_2025_FRA (Architecture v0001g)</t>
+  </si>
+  <si>
+    <t>Renommage des Définitions des jeux de propriétés ACA : 
+- ACA-JPPA-objet (pour les jeux personnalisés de propriétés applicables - JPPA) ;
+- ACA-Style-objet (pour les jeux de propriétés automatiques, hérités des styles d'objets ACA, notion qui n'existait pas jusqu'alors pour la modélisation traditionnelle avec Civil 3D)</t>
   </si>
 </sst>
 </file>
@@ -538,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D13BAD-6F1A-48D2-A554-8EAC8DE81690}">
-  <dimension ref="B2:C10"/>
+  <dimension ref="B2:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -612,6 +620,14 @@
         <v>14</v>
       </c>
     </row>
+    <row r="11" spans="2:3" ht="57" x14ac:dyDescent="0.45">
+      <c r="B11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Evolution du gabarit ACA en indice "H"
</commit_message>
<xml_diff>
--- a/ACA tool palettes/FRA/Gabarit ACA/Evolution du gabarit ACA.xlsx
+++ b/ACA tool palettes/FRA/Gabarit ACA/Evolution du gabarit ACA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin Marquette\Documents\GitHub\BetaProgram\ACA tool palettes\FRA\Gabarit ACA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D6A6DF-A18F-4385-A244-0021F42F96BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0601E6C4-8F91-4EBC-A950-D2E47E42F58E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17596" xr2:uid="{A80ABF4B-E54B-4375-B72F-5407CCC93B9D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>_C3D-TEMPLATE_2025_FRA (Architecture v0001a)</t>
   </si>
@@ -125,6 +125,12 @@
     <t>Renommage des Définitions des jeux de propriétés ACA : 
 - ACA-JPPA-objet (pour les jeux personnalisés de propriétés applicables - JPPA) ;
 - ACA-Style-objet (pour les jeux de propriétés automatiques, hérités des styles d'objets ACA, notion qui n'existait pas jusqu'alors pour la modélisation traditionnelle avec Civil 3D)</t>
+  </si>
+  <si>
+    <t>_C3D-TEMPLATE_2025_FRA (Architecture v0001h)</t>
+  </si>
+  <si>
+    <t>Modification des styles Plan pour les lignes de coupe de l'édifice (bleu) et les lignes d'élévation de l'édifice (magenta)</t>
   </si>
 </sst>
 </file>
@@ -546,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D13BAD-6F1A-48D2-A554-8EAC8DE81690}">
-  <dimension ref="B2:C11"/>
+  <dimension ref="B2:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -628,6 +634,14 @@
         <v>16</v>
       </c>
     </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>